<commit_message>
migrations and bugs fixed
</commit_message>
<xml_diff>
--- a/results/indicator_extract_1.xlsx
+++ b/results/indicator_extract_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B312"/>
+  <dimension ref="A1:B331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,3727 +453,3955 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Interventions are never one-dimensional. The interconnected nature of climate and project activities call for appropriate safeguarding mechanisms.</t>
+          <t>Interventions are never one-dimensional, and the interconnected nature of climate and project activities calls for appropriate safeguarding mechanisms to identify, prevent, and mitigate negative, unintended consequences.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1.1.2</t>
+          <t>1.1.4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The Gold Standard for the Global Goals (GS4GG) Safeguarding Principles &amp; Requirements is derived from several international conventions.</t>
+          <t>The requirements outlined in this document guide a project developer and its representatives to identify and evaluate the risks and adverse outcomes of the proposed activities and to adopt a mitigation strategy to avoid or minimize identified risks.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1.1.3</t>
+          <t>2.1.2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>This document outlines the overarching safeguarding principles and corresponding requirements that an activity is required to meet throughout the entire project cycle.</t>
+          <t>The project developer demonstrates full compliance with the requirements of this document for any activity for which the contract(s) between VVB and the project developer/Coordinating and Management Entity (CME) is signed on or after this standard enters into force.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1.1.4</t>
+          <t>2.1.3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>The requirements outlined in this document guide a project developer and its representatives to identify and evaluate the risks and adverse outcomes of the proposed activities, and to adopt a mitigation strategy to avoid, or where avoidance is not possible, minimise identified risks, to achieve the stated requirements.</t>
+          <t>Any project listed after the date of entry into force of this document follows the requirements of this document.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2.1.1</t>
+          <t>2.1.4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>The Version 2.1 of the Safeguarding Principles and Requirements enters into force 90 days after publication date i.e. 29 September 2023.</t>
+          <t>The project developer may voluntarily apply the requirements of this document to any new or ongoing activity for certification after its publication date.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2.1.2</t>
+          <t>4.1.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The project developer shall demonstrate full compliance with the requirements of this document for any activity for which the contract(s) between VVB and the project developer/Coordinating and Management Entity (CME) is signed on or after this standard enters into force.</t>
+          <t>All GS4GG project activities shall undertake upfront assessment against the Safeguarding Principles &amp; Requirements, implement the activity in accordance with the Safeguarding Principles and relevant requirements, include measures to minimize and address negative impacts in validated design documents prior to design certification, provide information on measures implemented to address the identified risks and status of risk in the monitoring report at each verification, and report any grievances related to compliance and safeguarding principles registered during the project cycle.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2.1.3</t>
+          <t>4.1.2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Any project listed after the date of entry into force of this document shall follow the requirements of this document.</t>
+          <t>The project complies with applicable national law, including those laws implementing host country obligations under international law, and when host country requirements differ from requirements presented in this document, projects comply with the more stringent requirements.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2.1.4</t>
+          <t>4.1.3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The project developer may voluntarily apply the requirements of this document to any new or ongoing activity for certification after its publication date.</t>
+          <t>The safeguarding assessment applies to the Project Scenario, although assessment questions and requirements involve a comparison to the Baseline Scenario(s) and/or the implementation or decommissioning phases of a Project.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4.1.1</t>
+          <t>4.1.4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>All GS4GG project activities/PoAs/VPAs shall undertake upfront assessment against the Safeguarding Principles &amp; Requirements, implement the activity in accordance with the Safeguarding Principles and relevant requirements, include measures to minimise and address negative impacts in validated design documents prior to design certification, provide information on measures implemented to address the identified risks and status of risk in the monitoring report at each verification, and report any grievances related to compliance and safeguarding principles that are registered at any point during the project cycle.</t>
+          <t>Any failure at any time in completion of the Safeguarding Principles Assessment, including nonconformity with Requirements and Monitoring &amp; Reporting Requirements, leads to invoking the Non-Conformity section of the Principles and Requirements.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4.1.2</t>
+          <t>4.2.1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The project shall comply with applicable national law, including those laws implementing host country obligations under international law, and when host country requirements differ from requirements presented in this document, projects shall comply with the requirements whichever is more stringent.</t>
+          <t>Where applicable, the project demonstrates that the Expert Stakeholder(s) has conducted a thorough review and that their recommendations have been incorporated into the project design.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4.1.3</t>
+          <t>5.1.1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>The safeguarding assessment shall apply to the Project Scenario, although assessment questions and requirements involve a comparison to the Baseline Scenario(s) and/or the implementation or decommissioning phases of a Project.</t>
+          <t>The Safeguarding Principles Assessment procedure set out in this document includes the following elements.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4.1.4</t>
+          <t>5.1.2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Any failure at any time in completion of the Safeguarding Principles Assessment, including nonconformity with Requirements and Monitoring &amp; Reporting Requirements shall lead to the invoking the Non-Conformity section of the Principles and Requirements.</t>
+          <t>A non-exhaustive list of assessment questions set out against each Safeguarding Principle is provided in the Annex 1.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4.1.5</t>
+          <t>6.1.1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>The activity shall provide the following information as per GS4GG certification stage as applicable to project status.</t>
+          <t>In certain circumstances, an exception to a specific Safeguarding Principle or Requirement may be sought.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4.2.1</t>
+          <t>P.1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Several Safeguarding Principles require the opinion and recommendations of independent Expert Stakeholder(s). Where applicable, demonstrate that the Expert Stakeholder(s) has conducted a thorough review and that their recommendations have been incorporated into the project design.</t>
+          <t>The Gold Standard recognizes the centrality of human rights to sustainable development and supports promoting and encouraging respect for human rights and for fundamental freedoms for all without distinction as to race, sex, language, or religion.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4.3.1</t>
+          <t>P.1.1.1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Evidence shall be provided to the validating and/or verifying body to demonstrate compliance with safeguarding principles and their requirements.</t>
+          <t>The project developer, its representatives, and the Project shall respect internationally proclaimed human rights and shall not be complicit in violence or human rights abuses of any kind as defined in the Universal Declaration of Human Rights.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4.3.2</t>
+          <t>P.1.1.2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>The necessary supporting documents and evidence shall be made available to Gold Standard as per the requirements of any findings raised during design review or performance review.</t>
+          <t>The Project shall not discriminate with regards to participation and inclusion.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4.3.3</t>
+          <t>P.1.1.3</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>The supporting documents and evidence shall be made publicly available on the Impact Registry except the confidential information or document in line with the Public Disclosure Requirements for Project Documentation.</t>
+          <t>The project shall not undermine the national or regional measures for the realisation of the right to development.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4.3.4</t>
+          <t>P.2.1.1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>If the supporting document or evidence contains confidential information, a redacted version of the same document shall be provided.</t>
+          <t>The Activity shall not directly or indirectly reinforce gender-based discrimination and shall not lead to or contribute to adverse impacts on gender equality and the situation of women.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5.1.1</t>
+          <t>P.2.1.2</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>The Safeguarding Principles Assessment procedure set out in this document includes the following elements.</t>
+          <t>Projects shall apply the principles of non-discrimination, equal treatment, and equal pay for equal work.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>P.1.1.1</t>
+          <t>P.2.1.3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>The project developer, its representatives, and the Project respect internationally proclaimed human rights and are not complicit in violence or human rights abuses of any kind as defined in the Universal Declaration of Human Rights.</t>
+          <t>The Project shall refer to the country’s national gender strategy or equivalent national commitment to aid in assessing gender risks.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>P.1.1.2</t>
+          <t>P.2.1.4</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>The Project does not discriminate with regards to participation and inclusion.</t>
+          <t>Gold Standard may require that the Project seek the input of an Expert Stakeholder(s) and to include their recommendations in the Project design.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>P.1.1.3</t>
+          <t>P.3.1.1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>The project does not undermine the national or regional measures for the realisation of the right to development.</t>
+          <t>The activity avoids community exposure to increased health risks and does not adversely affect the health of the workers and the community.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>P.2.1.1</t>
+          <t>P.3.1.2</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>The Activity shall not directly or indirectly reinforce gender-based discrimination and shall not lead to/contribute to adverse impacts on gender equality and/or the situation of women.</t>
+          <t>The project undertakes appropriate health and safety assessment considering safety risks to communities, adopts appropriate avoidance, minimisation, and mitigation measures, and ensures accidents or incidents are appropriately recorded, reported, and addressed with emergency preparedness and response plans in place.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>P.2.1.2</t>
+          <t>P.3.1.3</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Projects shall apply the principles of non-discrimination, equal treatment, and equal pay for equal work.</t>
+          <t>The assessment and adopted management measures take into account differences in risk exposure and sensitivity of women and men, as well as marginalised and disadvantaged groups.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>P.2.1.3</t>
+          <t>P.3.1.4</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>The Project shall refer to the country’s national gender strategy or equivalent national commitment to aid in assessing gender risks.</t>
+          <t>The project puts measures in place to protect workers from inherent risks of the nature of their work/sector, including physical, chemical, biological, and radiological hazards.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>P.2.1.4</t>
+          <t>P.4.1.1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Based on the responses to requirements above, Gold Standard may require that the Project seek the input of an Expert Stakeholder(s) and to include their recommendations in the Project design.</t>
+          <t>The Project shall not involve or be complicit in the alteration, damage, or removal of any sites, objects, or structures of significant cultural heritage.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>P.3.1.1</t>
+          <t>P.4.1.1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>The activity avoids community exposure to increased health risks and disease and does not adversely affect the health of the workers and the community.</t>
+          <t>The Project shall not involve or be complicit in the alteration, damage, or removal of any sites, objects, or structures of significant cultural heritage.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>P.3.1.2</t>
+          <t>P.4.1.2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>The project undertakes appropriate health and safety assessment considering safety risks to communities, adopts appropriate avoidance, minimisation, and mitigation measures following national legal requirements and good international practice, and ensures accidents or incidents associated with projects are appropriately recorded, reported, and addressed, with emergency preparedness and response plans in place.</t>
+          <t>Where a Project proposes to utilise Cultural Heritage, affected communities shall be informed of their rights under Applicable Law, the scope and nature of the proposed commercial development, and the potential consequences of such development.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>P.3.1.3</t>
+          <t>P.4.1.3</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>The assessment and adopted management measures take into account differences in risk exposure and sensitivity of women and men, as well as marginalised and disadvantaged groups, including children, older persons, persons with disabilities, minorities, and indigenous people.</t>
+          <t>The Project shall provide for equitable sharing of benefits from commercialisation of such knowledge, innovation, or practice, consistent with their customs and traditions.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>P.3.1.4</t>
+          <t>P.4.1.4</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>The project puts measures in place to protect workers from inherent risk of the nature of their work/sector including but not limited to physical, chemical, biological and radiological hazards, and specific threats to women.</t>
+          <t>The opinions and recommendations of an Expert Stakeholder(s) shall be sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>P.4.1.1</t>
+          <t>P.4.2.1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>The Project shall not involve or be complicit in the alteration, damage, or removal of any sites, objects, or structures of significant cultural heritage.</t>
+          <t>The Project shall not involve and shall not be complicit in the involuntary relocation of people.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>P.4.1.1</t>
+          <t>P.4.2.2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>The Project shall not involve or be complicit in the alteration, damage, or removal of any sites, objects, or structures of significant cultural heritage.</t>
+          <t>Projects shall avoid physical and economic displacement and mitigate displacement impacts and risks of displaced persons and host communities, integrating a resettlement Action Plan and/or Livelihood Action Plan into the Project documentation when displacement cannot be avoided.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>P.4.1.2</t>
+          <t>P.4.2.3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Where a Project proposes to utilise Cultural Heritage, including the knowledge, innovations, or practices of local communities, affected communities shall be informed of their rights under Applicable Law, the scope and nature of the proposed commercial development, and the potential consequences of such development.</t>
+          <t>The opinions and recommendations of an Expert Stakeholder(s) shall be sought and demonstrated as being included in the project design, where a project involves physical or economic displacement.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>P.4.1.3</t>
+          <t>P.4.3.1</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>The Project shall provide for equitable sharing of benefits from commercialisation of such knowledge, innovation, or practice, consistent with their customs and traditions.</t>
+          <t>The Project shall identify all such sites/matters such as reform.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>P.4.1.4</t>
+          <t>P.4.3.1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>The opinions and recommendations of an Expert Stakeholder(s) shall be sought and demonstrated as being included in the project design.</t>
+          <t>The Project identifies all sites/matters such as reform, modification, regularisation, redistribution, recording, registration, or inventory of legitimate tenure rights potentially affected by the Project and respects and safeguards legal rights, customary rights, and special cultural, ecological, economic, religious, or spiritual significance of people.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>P.4.2.1</t>
+          <t>P.4.3.2</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>The Project shall not involve and shall not be complicit in the involuntary relocation of people.</t>
+          <t>Changes in legal arrangements are in line with relevant laws and regulations, carried out in strict adherence with such laws, and all legal disputes are resolved prior to the Project being carried out in such areas, with changes demonstrated as having been agreed with free, prior, and informed consent.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>P.4.2.2</t>
+          <t>P.4.3.3</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Projects shall avoid physical and economic displacement, and mitigate displacement impacts and risks of displaced persons and host communities, when displacement cannot be avoided. In such cases, the Project shall integrate into the Project documentation, a resettlement Action Plan and/or Livelihood Action Plan, as appropriate.</t>
+          <t>The project developer holds uncontested land title for the entire Project Boundary to complete Project Design Certification.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>P.4.2.3</t>
+          <t>P.4.3.4</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>The opinions and recommendations of an Expert Stakeholder(s) shall be sought and demonstrated as being included in the project design, where a project involves physical or economic displacement.</t>
+          <t>The opinions and recommendations of an Expert Stakeholder(s) are sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>P.4.3.1</t>
+          <t>P.4.3.5</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>The Project identifies all sites/matters such as reform, modification, regularisation, redistribution, recording, registration, or inventory of legitimate tenure rights potentially affected by the Project and respects and safeguards legal rights, customary rights, or special cultural, ecological, economic, religious, or spiritual significance of people.</t>
+          <t>The project provides means for the affected to voice their grievances, ensuring there is a functioning mechanism in place to receive, process, resolve, communicate, and record grievances.</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>P.4.3.2</t>
+          <t>P.4.4.1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Changes in legal arrangements are in line with relevant laws and regulations and are carried out in strict adherence with such laws. All legal disputes are resolved prior to the Project being carried out in such areas, and all such changes are demonstrated as having been agreed with free, prior, and informed consent.</t>
+          <t>The Project identifies all communities of Indigenous People within the Project area of influence who may be affected directly or indirectly by the Project.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>P.4.3.3</t>
+          <t>P.4.4.2</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>The project developer holds uncontested land title for the entire Project Boundary to complete Project Design Certification.</t>
+          <t>As part of the design process, the activity carries out an environmental and social analysis of the activities that may affect or involve Indigenous Peoples, verifying whether they reside in the proposed project areas and assessing potential impacts on their rights, lands, territories, gender relations, and resources.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>P.4.3.4</t>
+          <t>P.4.4.3</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>The opinions and recommendations of an Expert Stakeholder(s) are sought and demonstrated as being included in the project design.</t>
+          <t>The project does not result in the forced eviction of indigenous people from their lands and territories.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>P.4.3.5</t>
+          <t>P.4.4.4</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>The project provides means for the affected to voice their grievances ensuring there is a functioning mechanism in place to receive, process, resolve, communicate and record grievances.</t>
+          <t>The project developer recognizes and respects the indigenous people’s collective rights to own, use, develop, and control the lands, resources, and territories that they have traditionally owned, occupied, or otherwise used or acquired.</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>P.4.4.1</t>
+          <t>P.4.4.5</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>The Project identifies all communities of Indigenous People within the Project area of influence who may be affected directly or indirectly.</t>
+          <t>The project developer respects, protects, conserves, and does not take the cultural, intellectual, religious, and/or spiritual property of indigenous people without their free, prior, and informed consent (FPIC).</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>P.4.4.2</t>
+          <t>P.4.4.6</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>As part of the design process, the activity shall carry out an environmental and social analysis of the activities that may affect or involve Indigenous Peoples. The analysis shall verify whether Indigenous Peoples reside in the proposed project areas and/or if the activities may affect Indigenous Peoples outside of project areas. The assessment shall include the potential impacts on their rights, lands, territories, gender relations and resources.</t>
+          <t>The project developer ensures that the indigenous people are provided with equitable sharing of benefits derived from the utilization and/or commercial development of natural resources on their lands and territories or use of their traditional knowledge and practices.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>P.4.4.3</t>
+          <t>P.4.4.7</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>The project shall not result in the forced eviction of indigenous people from their lands and territories.</t>
+          <t>An 'Indigenous People Plan' (IPP) or 'Indigenous People Plan Framework' is elaborated and included in the project documentation in accordance with the effective and meaningful participation of indigenous peoples and UNDP Guidelines.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>P.4.4.4</t>
+          <t>P.4.4.8</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>The project developer shall recognise and respect the indigenous people’s collective rights to own, use, and develop and control the lands, resources and territories that they have traditionally owned, occupied or otherwise used or acquired, including lands and territories for which they do not yet possess title.</t>
+          <t>Projects make available mutually agreed, culturally appropriate, accessible, and inclusive channels for feedback and grievance redress to Indigenous Peoples and their representatives, with a grievance mechanism established at the beginning of programme or project implementation.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>P.4.4.5</t>
+          <t>P.4.4.9</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>The project developer shall respect, protect, conserve and shall not take the cultural, intellectual, religious, and/or spiritual property of indigenous people without their free, prior and informed consent (FPIC).</t>
+          <t>The opinions and recommendations of an Expert Stakeholder(s) are sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>P.4.4.6</t>
+          <t>P.5.1.1</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>The project developer shall ensure that the indigenous people are provided with the equitable sharing of benefits to be derived from utilisation and/or commercial development of natural resources on lands and territories or use of their traditional knowledge and practices by the Project. This shall be done in a manner that is culturally appropriate and inclusive and that does not impede land rights or equal access to basic services including health services, clean water, energy, education, safe and decent working conditions, and housing.</t>
+          <t>The Project does not involve, is not complicit in, or does not inadvertently contribute to or reinforce corruption or corrupt practices.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>P.4.4.7</t>
+          <t>P.6.1.1</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>If it is determined that the proposed project may affect the rights, lands, resources, or territories of indigenous people, an 'Indigenous People Plan' (IPP) or 'Indigenous People Plan Framework' shall be elaborated and included in the project documentation. This plan shall be developed in accordance with the effective and meaningful participation of indigenous peoples and in accordance with UNDP Guidelines.</t>
+          <t>The project developer ensures that there is no forced labour and that all employment is in compliance with national labour and occupational health and safety laws, with obligations under international law.</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>P.4.4.8</t>
+          <t>P.6.1.2</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Projects shall make available mutually agreed, culturally appropriate, accessible and inclusive channels for feedback and grievance redress to Indigenous Peoples and their representatives. The grievance mechanism shall be established at the beginning of programme or project implementation with due consideration given to customary dispute settlement mechanisms among the Indigenous Peoples concerned and remain operational throughout the project cycle. A conflict resolution mechanism should be also discussed, agreed and developed during the early stages of the programme or project cycle.</t>
+          <t>The employment decisions are based on the principle of equal opportunity and fair treatment.</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>P.4.4.9</t>
+          <t>b.i</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>The opinions and recommendations of an Expert Stakeholder(s) shall be sought and demonstrated as being included in the project design.</t>
+          <t>Working agreements with all individual workers are documented and implemented, comprising working hours that do not exceed 48 hours per week on a regular basis.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>P.5.1.1</t>
+          <t>b.ii</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>The Project shall not involve, be complicit in or inadvertently contribute to or reinforce corruption or corrupt practices.</t>
+          <t>Working agreements with all individual workers are documented and implemented, comprising duties and tasks.</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>P.6.1.1</t>
+          <t>b.iii</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>The project developer ensures that there is no forced labour and that all employment is in compliance with national labour and occupational health and safety laws, with obligations under international law, and consistency with the principles and standards embodied in the International Labour Organisation (ILO) fundamental conventions.</t>
+          <t>Working agreements with all individual workers are documented and implemented, comprising remuneration that includes provision for payment of overtime.</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>P.6.1.2</t>
+          <t>b.iv</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>The employment decisions are based on the principle of equal opportunity and fair treatment.</t>
+          <t>Working agreements with all individual workers are documented and implemented, comprising modalities on health insurance.</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>P.6.1.3</t>
+          <t>b.v</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>The project shall comply with national law, where national law provides provision to address non-discrimination in employment. When national laws are silent on non-discrimination in employment, the project shall meet the requirements outlined in this document. In circumstances where national law is inconsistent with this Standard, the project developer is encouraged to carry out its operations consistent with the intent of paragraph P.6.1.2 above without contravening applicable laws.</t>
+          <t>Working agreements with all individual workers are documented and implemented, comprising modalities on termination of the contract with provision for voluntary resignation by employee.</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>P.6.1.4</t>
+          <t>b.vi</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Child labour, as defined by the ILO Minimum Age Convention (No. 138) and ILO Worst Forms of Child Labour Convention, 1999, (No. 182) is not allowed. The project developer shall use adequate and verifiable mechanisms for age verification in recruitment procedures and validated and verified by VVB.</t>
+          <t>Working agreements with all individual workers are documented and implemented, comprising provision for annual leave of not less than 10 days per year, not including sick and casual leave.</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>P.6.1.5</t>
+          <t>b.vii</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>A child under the age of eighteen shall not perform work in connection with or arising from the activities which, by its nature or the circumstances in which it is carried out, is likely to harm his/her health, safety or morals. Such work is determined by national laws or regulations or by the competent authority and commonly specified in national lists of hazardous work prohibited to children. In the absence of such regulations, guidance on hazardous work to be prohibited in connection with the project should derive from the relevant ILO instruments.</t>
+          <t>Working agreements with all individual workers are documented and implemented, comprising provision for maternity leave, vacation, or holidays.</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>P.6.1.6</t>
+          <t>c</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Exceptions are children for work on their families’ property as long as their compulsory schooling is not hindered, the tasks they perform do not harm their development, and the opinions and recommendations of an Expert Stakeholder are sought and included in the project design.</t>
+          <t>Where such agreements do not exist or do not address working conditions and terms of employment, the project developer provides reasonable working conditions and terms of employment.</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>P.6.1.7</t>
+          <t>d</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>The project developer implements necessary processes and measures that address the safety and health of project workers to support project design, planning, and implementation.</t>
+          <t>Where migrant workers are engaged, the project developer ensures that they are engaged on substantially equivalent terms and conditions to non-migrant workers carrying out similar work.</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>P.6.1.8</t>
+          <t>e</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>The project developer and relevant parties who employ or engage project workers shall put in place safety and health processes and measures to prevent and protect workers from chemical, physical, biological, and psychosocial hazards and to establish and maintain safe and healthy workplaces including the work environment, organisation, processes, tools machinery and equipment.</t>
+          <t>Where accommodation services are provided to workers, the project developer puts in place and implements policies on the quality and management of the accommodation and provision of basic services.</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>P.6.1.9</t>
+          <t>P.6.1.3</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>The project developer shall implement appropriate measures to protect and provide assistance to address the vulnerabilities of project workers, including specific groups of workers, such as women, persons with disabilities, migrant workers, and young workers, and to prevent and address any form of violence and harassment, bullying, intimidation and/or exploitation, including any form of gender-based violence (GBV).</t>
+          <t>The project complies with national law regarding non-discrimination in employment.</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>P.6.1.10</t>
+          <t>P.6.1.4</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>In accordance to the GS4GG stakeholder engagement requirements, the project developer shall provide access to workers (and their organisations, where they exist) to grievance mechanism to raise workplace concerns of violations of existing rights and entitlements as provided for in legislation, collective agreements, employment contracts and human resources policies. The project developer shall inform the workers of the grievance mechanism at the time of recruitment and make accessible to them. Measures shall be put in place to make the grievance mechanism easily accessible to all workers.</t>
+          <t>Child labour, as defined by the ILO Minimum Age Convention and ILO Worst Forms of Child Labour Convention, is not allowed.</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>P.6.1.11</t>
+          <t>P.6.1.5</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Where project workers are engaged by third parties, the project developer shall put in place mechanism e.g. due diligence that includes an examination of the past and current labour practices of the contractor or third party, and audits to ascertain that third parties who engage workers are legitimate and reliable and have in place appropriate policies, processes and systems that allow them to operate in accordance with the minimum requirements herein, and establish policies and procedures for managing and monitoring the performance of such third-party employers in relation to the minimum requirements herein.</t>
+          <t>A child under the age of eighteen does not perform work in connection with project activities that is likely to harm his/her health, safety, or morals.</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>P.6.1.12</t>
+          <t>P.6.1.6</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Where project’s primary suppliers (supply chain workers) are involved, in a sector known for involving child or forced labour or significant safety violations, the project developer shall.</t>
+          <t>Exceptions are children for work on their families’ property as long as their compulsory schooling is not hindered, the tasks they perform do not harm their physical, mental, spiritual, moral, or social development, and the opinions and recommendations of an Expert Stakeholder are sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>P.6.2.1</t>
+          <t>P.6.1.7</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>The project developer ensures the financial sustainability of the Project implemented, including those that will occur beyond the project certification period.</t>
+          <t>The project developer implements necessary processes and measures that address the safety and health of project workers to support project design, planning, and implementation.</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>P.6.2.2</t>
+          <t>P.6.1.8</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>The Projects consider economic impacts and potential risks to the local economy, with particular attention to vulnerable and marginalised social groups in targeted communities, ensuring that benefits are socially inclusive and sustainable.</t>
+          <t>The project developer and relevant parties who employ or engage project workers put in place safety and health processes and measures to prevent and protect workers from hazards and to establish and maintain safe and healthy workplaces.</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>P.7.1.1</t>
+          <t>P.6.1.9</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Projects do not increase greenhouse gas emissions (GHG) over the Baseline Scenario unless specifically allowed within Activity Requirements or Gold Standard approved SDG impact quantification methodologies.</t>
+          <t>The project developer implements appropriate measures to protect and provide assistance to address the vulnerabilities of project workers, including specific groups of workers, and to prevent and address any form of violence and harassment.</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>P.7.2.1</t>
+          <t>P.6.1.10</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>The Project does not affect the availability and reliability of energy supply to other users.</t>
+          <t>The project developer provides access to workers to a grievance mechanism to raise workplace concerns and informs the workers of the grievance mechanism at the time of recruitment.</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>P.8.1.1</t>
+          <t>P.6.1.11</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>The Project ensures that water resources are conserved.</t>
+          <t>The project developer puts in place mechanisms to examine the past and current labour practices of third parties and establishes policies and procedures for managing and monitoring the performance of such third-party employers.</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>P.8.1.2</t>
+          <t>P.6.1.12</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>The opinions and recommendations of Expert Stakeholder(s) that help demonstrate compliance with the above are included in the project design and monitoring plan, where a risk exists.</t>
+          <t>The project developer ensures that where primary suppliers are involved in sectors known for child or forced labour or significant safety violations, appropriate measures are taken.</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>P.8.2.1</t>
+          <t>P.6.2.1</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>The risk of the Project negatively impacting the catchment is assessed and addressed.</t>
+          <t>The project developer ensures the financial sustainability of the Project implemented, including those that will occur beyond the project certification period.</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>P.8.2.1</t>
+          <t>P.6.2.2</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>The risk of the Project negatively impacting the catchment is assessed and addressed.</t>
+          <t>The Projects consider economic impacts and potential risks to the local economy, giving particular attention to vulnerable and marginalized social groups in targeted communities, ensuring that benefits are socially inclusive and sustainable.</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>P.8.2.2</t>
+          <t>P.7.1.1</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>The Project demonstrates that measures will be undertaken to ensure that surface and ground waters are protected from erosion and that these measures are in place prior to the commencement of the Project.</t>
+          <t>Projects do not increase greenhouse gas emissions (GHG) over the Baseline Scenario unless specifically allowed within Activity Requirements or Gold Standard approved SDG impact quantification methodologies.</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>P.8.2.3</t>
+          <t>P.7.2.1</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>The Project demonstrates that measures to ensure soil protection and minimised erosion are in place prior to the commencement of the Project.</t>
+          <t>The Project does not affect the availability and reliability of energy supply to other users.</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>P.8.2.4</t>
+          <t>P.8.1.1</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Measures are incorporated to reduce soil erosion on slopes, taking into account the concept of the effective slope length.</t>
+          <t>The Project ensures that water resources are conserved.</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>P.8.2.5</t>
+          <t>P.8.1.2</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>The success of measures is reassessed at a frequency appropriate to the context of the ecosystem affected.</t>
+          <t>The opinions and recommendations of Expert Stakeholder(s) that help demonstrate compliance with the above are included in the project design and monitoring plan, where a risk exists.</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>P.8.2.6</t>
+          <t>P.8.2.1</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>The opinions and recommendations of Expert Stakeholder(s) that help demonstrate compliance with the above are included in the project design and monitoring plan.</t>
+          <t>The risk of the Project negatively impacting the catchment is assessed and addressed.</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>P.9.1.1</t>
+          <t>P.8.2.2</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>The Project identifies the functions and services provided by the landscape and demonstrates no net degradation of soil resources and the loss of ecosystem services provided by soils.</t>
+          <t>The Project demonstrates that measures will be undertaken to ensure the catchment is protected.</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>P.9.1.2</t>
+          <t>P.8.2.1</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>To ensure healthy soil, appropriate measures are put in place to minimise adverse impacts on soil, their biodiversity, organic content, productivity, structure, and water-retention capacity.</t>
+          <t>The risk of the Project negatively impacting the catchment is assessed and addressed.</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>P.9.1.3</t>
+          <t>P.8.2.2</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Measures are incorporated to minimise soil degradation.</t>
+          <t>The Project demonstrates that measures will be undertaken to ensure that surface and ground waters are protected from erosion and that these measures are in place prior to the commencement of the Project.</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>P.9.1.4</t>
+          <t>P.8.2.3</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Projects that involve the production, harvesting, and/or management of living natural resources by small-scale landholders and/or local communities adopt the appropriate and culturally sensitive sustainable resource management practices.</t>
+          <t>The Project demonstrates that measures to ensure soil protection and minimised erosion are in place prior to the commencement of the Project.</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>P.9.2.1</t>
+          <t>P.8.2.4</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>The Project avoids or minimises the exacerbation of impacts caused by natural or man-made hazards, such as landslides or floods that could result from land use changes due to Projects.</t>
+          <t>Measures are incorporated to reduce soil erosion on slopes, taking into account the concept of the effective slope length.</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>P.9.2.2</t>
+          <t>P.8.2.5</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>The project developer includes mitigation measures (if possible), the emergency preparedness plan and response strategies.</t>
+          <t>The success of measures is reassessed at a frequency appropriate to the context of the ecosystem affected.</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>P.9.3.1</t>
+          <t>P.8.2.6</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>The projects that may involve the transfer, handling, and use of genetically modified organisms/living modified organisms (GMOs/LMOs) that result from modern biotechnology and that may have adverse effects on biological diversity, the project developer ensures that a risk assessment by a competent Expert stakeholder is carried out in accordance with Annex III of the Cartagena Protocol on Biosafety to the Convention on Biological Diversity.</t>
+          <t>The opinions and recommendations of Expert Stakeholder(s) that help demonstrate compliance with the above are included in the project design and monitoring plan.</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>P.9.3.2</t>
+          <t>P.9.1.1</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>The project developer ensures that projects involving GMOs/LMOs include measures to manage any risks identified in the risk assessment.</t>
+          <t>The Project identifies the functions and services provided by the landscape and demonstrates no net degradation of soil resources and the loss of ecosystem services provided by soils.</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>P.9.3.3</t>
+          <t>P.9.1.2</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Forestry projects (for example Afforestation/Reforestation) involving GMO planting are not eligible for Certification under Gold Standard for the Global Goals.</t>
+          <t>To ensure healthy soil, appropriate measures are put in place to minimise adverse impacts on soil, their biodiversity, organic content, productivity, structure, and water-retention capacity.</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>P.9.4.1</t>
+          <t>P.9.1.3</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>The Project avoids the release of pollutants from routine, non-routine, and accidental releases. If emissions cannot be avoided, the project minimizes and controls the intensity and flow. This applies to the release of pollutants to air, water, and land due to routine, non-routine, and accidental circumstances.</t>
+          <t>Measures are incorporated to minimise soil degradation through practices such as crop rotation, composting, and reduced tillage.</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>P.9.4.2</t>
+          <t>P.9.1.4</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>The project developer ensures that pollution prevention and control technologies and practices consistent with national regulation or international good practice are applied during the Project life cycle.</t>
+          <t>Projects involving the production, harvesting, and/or management of living natural resources by small-scale landholders and/or local communities adopt appropriate and culturally sensitive sustainable resource management practices.</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>P.9.4.3</t>
+          <t>P.9.2.1</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>All potential pollution sources that may result from the Project that cause the degradation of the quality of soil, air, surface, and groundwater within the Project’s area of influence are identified. Appropriate mitigation measures and monitoring are implemented to ensure the protection of resources.</t>
+          <t>The Project avoids or minimises the exacerbation of impacts caused by natural or man-made hazards, such as landslides or floods that could result from land use changes due to Projects.</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>P.9.5.1</t>
+          <t>P.9.2.2</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>The project developer avoids the generation of hazardous and non-hazardous waste materials and implements a waste management hierarchy that prioritizes the avoidance of waste generation.</t>
+          <t>The project developer includes mitigation measures, the emergency preparedness plan, and response strategies.</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>P.9.5.2</t>
+          <t>P.9.3.1</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>If the generated waste is considered hazardous, reasonable alternatives for its environmentally sound disposal are adopted while adhering to the limitations applicable to its transboundary movement.</t>
+          <t>The project developer ensures that a risk assessment by a competent Expert stakeholder is carried out in accordance with Annex III of the Cartagena Protocol on Biosafety to the Convention on Biological Diversity for projects involving GMOs/LMOs.</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>P.9.5.3</t>
+          <t>P.9.3.2</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Projects avoid or, when avoidance is not feasible, minimize and control the release of hazardous materials resulting from their production, transportation, handling, storage, and use.</t>
+          <t>The project developer ensures that projects involving GMOs/LMOs include measures to manage any risks identified in the risk assessment.</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>P.9.5.4</t>
+          <t>P.9.3.3</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Projects consider the use of less hazardous substitutes for such chemicals and materials and avoid the manufacture, trade, and use of hazardous materials.</t>
+          <t>Forestry projects involving GMO planting are not eligible for Certification under Gold Standard for the Global Goals.</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>P.9.5.4</t>
+          <t>P.9.4.1</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Projects shall consider the use of less hazardous substitutes for chemicals and materials and shall avoid the manufacture, trade, and use of chemicals and hazardous materials subject to international bans or phase-outs due to their high toxicity to living organisms, environmental persistence, potential for bioaccumulation, or potential for depletion of the ozone layer, unless for acceptable purposes as defined by the conventions or protocols.</t>
+          <t>The project avoids the release of pollutants from routine, non-routine, and accidental releases, and minimizes and controls the intensity and flow of emissions that cannot be avoided.</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>P.9.5.5</t>
+          <t>P.9.4.2</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>The Project shall not make use of chemicals or materials subject to international bans or phase-outs.</t>
+          <t>The project developer ensures that pollution prevention and control technologies and practices consistent with national regulation or international good practice are applied during the Project life cycle.</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>P.9.6.1</t>
+          <t>P.9.4.3</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>For activities involving pest management, the integrated pest management (IPM) and/or integrated vector management (IVM) approaches shall be adopted and aim to reduce reliance on chemical pesticides. A Pest Management Plan shall be developed where use of a significant volume of pesticides is foreseen, to demonstrate how IPM/IVM is promoted to reduce reliance on pesticides and describe measures to minimise risks of pesticide use.</t>
+          <t>All potential pollution sources that may result from the Project that cause the degradation of the quality of soil, air, surface, and groundwater within the Project’s area of influence are identified, and appropriate mitigation measures and monitoring are implemented.</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>P.9.6.2</t>
+          <t>P.9.5.1</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>The health and environmental risks associated with pest management should be minimised with support, as needed, to institutional capacity development, to help regulate and monitor the distribution and use of pesticides and enhance the application of integrated pest management.</t>
+          <t>The project developer shall avoid the generation of hazardous and non-hazardous waste materials and implement a waste management hierarchy that prioritizes the avoidance of the generation of waste.</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>P.9.6.3</t>
+          <t>P.9.5.1.a</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>When projects include pest management or the use of chemical pesticides, pesticides that are low in human toxicity, known to be effective against the target species, and have minimal effects on non-target species and the environment shall be selected. When the project developer selects chemical pesticides, the selection shall be based upon requirements that the pesticides be packaged in safe containers, be clearly labelled for safe and proper use, and that the pesticides have been manufactured by an entity currently licensed by relevant regulatory agencies.</t>
+          <t>The project shall minimize waste generation and wastes shall be recovered, recycled, and reused in a safe manner.</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>P.9.6.4</t>
+          <t>P.9.5.1.b</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>There shall be a ‘Chemical Pesticides Policy’ that is documented, implemented, and regularly updated. This policy shall include at a minimum provisions for safe transport, storage, handling, and application, and provisions for emergency situations.</t>
+          <t>Where waste may not be recovered or reused, it shall be treated, destroyed, or disposed of in an environmentally sound manner that includes the appropriate control of emissions and residues resulting from the handling and processing of the waste material.</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>P.9.6.5</t>
+          <t>P.9.5.2</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>The project developer shall not purchase, store, manufacture, trade or use products that fall in Classes IA (extremely hazardous) and IB (highly hazardous) of the World Health Organization Recommended Classification of Pesticides by Hazard. The project developer shall not purchase, store, use, manufacture, or trade in Class II (moderately hazardous) pesticides, unless the project has appropriate controls on manufacture, procurement, or distribution and/or use of these chemicals. These chemicals shall not be accessible to personnel without proper training, equipment, and facilities to handle, store, apply, and dispose of these products properly.</t>
+          <t>If the generated waste is considered hazardous, reasonable alternatives for its environmentally sound disposal shall be adopted while adhering to the limitations applicable to its transboundary movement.</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>P.9.6.6</t>
+          <t>P.9.5.3</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Fertilisers shall be avoided, or fertiliser use shall be minimised to ensure the effective and efficient use of fertilisers to meet agricultural demands while minimising nutrient losses to the environment. The project developer should put measures in place to preserve ecosystem services and minimise environmental impacts from the use of fertilisers including soil and water pollution, ammonia volatilisation, greenhouse gas emissions, and other nutrient loss mechanisms.</t>
+          <t>Projects shall avoid or, when avoidance is not feasible, minimize and control the release of hazardous materials resulting from their production, transportation, handling, storage, and use.</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>P.9.7.1</t>
+          <t>P.9.5.3</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>The project enhances the sustainable management of forests, including the application of independent, credible certification for commercial, industrial-scale timber harvesting, maintains or enhances biodiversity and ecosystem functionality in areas where improved forest management is undertaken, and ensures that plantations are environmentally appropriate, socially beneficial, and economically viable, utilizing native species wherever feasible.</t>
+          <t>The health risks, including potential differentiated effects on men, women, and children, of the potential use of hazardous materials shall be addressed appropriately.</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>P.9.7.2</t>
+          <t>P.9.5.4</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>The project applying Land Use &amp; Forest Activity requirements complies with additional safeguarding requirements, as applicable.</t>
+          <t>Projects shall consider the use of less hazardous substitutes for such chemicals and materials and shall avoid the manufacture, trade, and use of hazardous materials.</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>P.9.8.1</t>
+          <t>P.9.5.4</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>The activity shall not negatively influence access to and availability of food for people affected.</t>
+          <t>Projects consider the use of less hazardous substitutes for chemicals and materials and avoid the manufacture, trade, and use of chemicals and hazardous materials subject to international bans or phase-outs due to their high toxicity to living organisms, environmental persistence, potential for bioaccumulation, or potential for depletion of the ozone layer.</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>P.9.9.1</t>
+          <t>P.9.5.5</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>The welfare of animals is ensured by provision of sufficient access to drinking water and adequate food, access to daylight, providing appropriate environment including shelter and a comfortable resting area, providing humane treatment during handling and slaughter or killing, no hindrance in their sensory perception and performing their basic needs, prohibition of cattle trainers, and management policies and staff training to prevent mistreatment.</t>
+          <t>The Project does not make use of chemicals or materials subject to international bans or phase-outs.</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>P.9.9.2</t>
+          <t>P.9.6.1</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Excessive or inadequate use of veterinary medicines is avoided, and all medications are administered strictly according to label and package instructions or according to a trained veterinarian.</t>
+          <t>For activities involving pest management, the integrated pest management (IPM) and/or integrated vector management (IVM) approaches are adopted and aim to reduce reliance on chemical pesticides, and a Pest Management Plan is developed where use of a significant volume of pesticides is foreseen.</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>P.9.9.3</t>
+          <t>P.9.6.2</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Injured or sick animals are treated and isolated, if necessary, for recovery, and control measures are put in place to ensure the transfer of disease (especially of zoonotic nature) is minimized.</t>
+          <t>The health and environmental risks associated with pest management are minimised with support, as needed, to institutional capacity development, to help regulate and monitor the distribution and use of pesticides and enhance the application of integrated pest management.</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>P.9.9.4</t>
+          <t>P.9.6.3</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Synthetic growth promoters including hormones are not administered.</t>
+          <t>When Projects include pest management or the use of chemical pesticides, measures are taken to minimise risks of pesticide use.</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>P.9.9.5</t>
+          <t>P.9.6.3</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Animals are handled using low-stress methods, equipment, and facilities that facilitate calm animal movement.</t>
+          <t>When projects include pest management or the use of chemical pesticides, pesticides that are low in human toxicity, known to be effective against the target species and have minimal effects on non-target species and the environment shall be selected.</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>P.9.9.6</t>
+          <t>P.9.6.4</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Animals are exposed to the least stress possible during transportation and slaughtering.</t>
+          <t>There shall be a ‘Chemical Pesticides Policy’ that is documented, implemented, and regularly updated, including provisions for safe transport, storage, handling, and application, and provisions for emergency situations.</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>P.9.9.7</t>
+          <t>P.9.6.5</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Appropriate space per animal and stocking rates per land unit are set according to their developmental and physical needs.</t>
+          <t>The project developer shall not purchase, store, manufacture, trade or use products that fall in Classes IA (extremely hazardous) and IB (highly hazardous) of the World Health Organization Recommended Classification of Pesticides by Hazard, and shall not purchase, store, use, manufacture, or trade in Class II (moderately hazardous) pesticides unless appropriate controls are in place.</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>P.9.9.8</t>
+          <t>P.9.6.6</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>For projects involving aquatic animals, special attention is paid to their specific needs, including flow, quantity, and quality of water supply, and quantities of feed and required nutritional composition for the farmed animals.</t>
+          <t>Fertilisers shall be avoided, or fertiliser use shall be minimised to ensure effective and efficient use while minimising nutrient losses to the environment, with measures in place to preserve ecosystem services and minimise environmental impacts.</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>P.9.9.9</t>
+          <t>P.9.7.1</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Activity that involves primary production of living natural resources, such as animal husbandry, aquaculture, and fisheries, shall implement sustainable management practices through the application of industry-specific good management practices and available technologies.</t>
+          <t>The project enhances the sustainable management of forests, including the application of independent, credible certification for commercial, industrial-scale timber harvesting, maintains or enhances biodiversity and ecosystem functionality in areas where improved forest management is undertaken, and ensures that plantations are environmentally appropriate, socially beneficial, and economically viable, utilizing native species wherever feasible.</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>P.9.9.10</t>
+          <t>P.9.8.1</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>The animal welfare standards are based firmly on scientific knowledge and practical experience, and compliance with the above paragraphs in the same section may require changes to husbandry practices. The project developer takes into account the animal welfare-related cultural practices of certain individuals and groups.</t>
+          <t>The activity does not negatively influence access to and availability of food for people affected.</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>P.9.10.1</t>
+          <t>P.9.9.1</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>No Project that potentially impacts identified habitats such as HCV areas and or Critical habitats shall be implemented unless all specified conditions are demonstrated.</t>
+          <t>The welfare of animals is ensured by providing sufficient access to drinking water and adequate food, access to daylight, an appropriate environment including shelter and a comfortable resting area, humane treatment during handling and slaughter or killing, no hindrance in their sensory perception and performing their basic needs, prohibition of cattle trainers, and management policies and staff training to prevent mistreatment.</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>P.9.10.2</t>
+          <t>P.9.9.2</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Within the Project, the area managed by the project developer and the area of impact downstream shall be identified and protected/enhanced, ensuring mitigation is in place within the Project Boundary.</t>
+          <t>Excessive or inadequate use of veterinary medicines is avoided, and all medications are administered strictly according to label and package instructions or according to a trained veterinarian.</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>P.9.10.3</t>
+          <t>P.9.9.3</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>If the Project is located in such habitats, the project developer shall minimise unwarranted conversion or degradation of the habitat and identify opportunities to enhance the habitat as part of the Project.</t>
+          <t>Injured or sick animals are treated and isolated, if necessary, for recovery, and control measures are put in place to ensure the transfer of disease, especially of zoonotic nature, is minimized.</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>P.9.10.4</t>
+          <t>P.9.9.4</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>For Activities applying the Land Use &amp; Forest Activity Requirements Projects, a minimum 10% of the Project area shall be identified and managed to protect or enhance the biological diversity of native ecosystems following HCV approach.</t>
+          <t>Synthetic growth promoters including hormones are not administered.</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>P.9.10.5</t>
+          <t>P.9.9.5</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>The opinions and recommendations of an Expert Stakeholder are sought and demonstrated as being included in the Project design.</t>
+          <t>Animals are handled using low-stress methods, equipment, and facilities that facilitate calm animal movement.</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>P.9.11.1</t>
+          <t>P.9.9.6</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Under no circumstances shall the Project lead to the reduction or negative impact of any recognised Endangered, Vulnerable or Critically Endangered species.</t>
+          <t>Animals are exposed to the least stress possible during transportation and slaughtering.</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>P.9.11.2</t>
+          <t>P.9.9.7</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Habitats of endangered species are specifically identified and managed to protect or enhance them.</t>
+          <t>Appropriate space per animal and stocking rates per land unit are set according to their developmental and physical needs.</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>P.9.11.3</t>
+          <t>P.9.9.8</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>The opinions and recommendations of an Expert Stakeholder are sought and demonstrated as being considered and incorporated into the project design.</t>
+          <t>The project that involves aquatic animals pays special attention to their specific needs regarding flow, quantity, and quality of water supply, and quantities of feed and required nutritional composition for the farmed.</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>P.9.12.1</t>
+          <t>P.9.10.1.a</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>The project under no circumstances shall introduce any alien species into new environments. The project shall not deliberately introduce any alien species with a high risk of invasive behaviour and shall implement measures to avoid accidental or unintended introductions.</t>
+          <t>The risk of the Project negatively impacting the catchment and risks impacting project success is assessed and addressed to ensure its ongoing, long-term viability and impact on surrounding HCV and ecological assets.</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>P.9.12.2</t>
+          <t>P.9.10.1.b</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Where alien species are already established in the country or region of the proposed project, the project developer shall exercise diligence in not spreading them into areas in which they have not already been established. The project developer should take measures to eradicate such species from the natural habitats over which they have management control.</t>
+          <t>There are no measurable adverse impacts on the criteria or biodiversity values for which the critical habitat was designated, and on the ecological processes supporting those biodiversity values.</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>P.1.1.1</t>
+          <t>P.9.10.1.c</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>The project developer, its representatives, and the Project do not disrespect internationally proclaimed human rights.</t>
+          <t>A robust, appropriately designed, and long-term Habitats and Biodiversity Action Plan is in place to achieve net gains of those biodiversity values for which the critical habitat was designated.</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>P.1.1.1</t>
+          <t>P.9.10.2.a</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>The project is not involved or complicit in violence or human rights abuses of any kind as defined in the Universal Declaration of Human Rights.</t>
+          <t>Existing patches of native tree species are identified and protected/enhanced within the Project.</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>P.1.1.2</t>
+          <t>P.9.10.2.b</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Local communities or individuals have not raised human rights concerns regarding the project.</t>
+          <t>Single solitary stems of native tree species are identified and protected/enhanced within the Project.</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>P.1.1.3</t>
+          <t>P.9.10.2.c</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>There is no risk that rights-holders do not have the capacity to claim their rights.</t>
+          <t>All freshwater resources including rivers, lakes, swamps, ephemeral water bodies, and wells are identified and protected/enhanced within the Project.</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>P.1.1.3</t>
+          <t>P.9.10.2.d</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>This project does not undermine national or regional measures for the realisation of the right to development.</t>
+          <t>Habitats of rare, threatened, and endangered species are identified and protected/enhanced within the Project.</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>P.1.1.1</t>
+          <t>P.9.10.2.e</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>The project does not potentially involve or lead to adverse impacts on enjoyment of the human rights of the affected population and particularly of marginalised groups.</t>
+          <t>Areas relevant for habitat connectivity are identified and protected/enhanced within the Project.</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>P.1.1.2</t>
+          <t>P.9.10.3.a</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>The project does not potentially involve or lead to inequitable or discriminatory impacts on affected populations, particularly people living in poverty or marginalised or excluded individuals or groups, including persons with disabilities.</t>
+          <t>Unwarranted conversion or degradation of the habitat is minimized by the project developer.</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>P.1.1.3</t>
+          <t>P.9.10.3.b</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>There are restrictions in availability, quality of and/or access to resources or basic services, in particular to marginalised individuals or groups, including persons with disabilities.</t>
+          <t>Opportunities to enhance the habitat are identified as part of the Project.</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>P.1.1.3</t>
+          <t>P.9.10.4</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>There is exacerbation of conflicts among and/or the risk of violence to project-affected communities and individuals.</t>
+          <t>A minimum of 10% of the Project area is identified and managed to protect or enhance the biological diversity of native ecosystems following the HCV approach.</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>P.2.1.1</t>
+          <t>P.9.11.1</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Women's groups/leaders have raised gender equality concerns regarding the project, (e.g., during the stakeholder engagement process, grievance processes, public statements).</t>
+          <t>The project does not lead to the reduction or negative impact of any recognised Endangered, Vulnerable or Critically Endangered species.</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>P.2.1.2</t>
+          <t>P.9.11.2</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>The project undermines the principles of non-discrimination, equal treatment, and equal pay for equal work.</t>
+          <t>Habitats of endangered species are specifically identified and managed to protect or enhance them.</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>P.2.1.2</t>
+          <t>P.9.11.3</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>The project prevents men and women from having equal opportunities to participate in identified tasks and activities, whether through paid work, volunteer work, or community contributions, as appropriate.</t>
+          <t>The opinions and recommendations of an Expert Stakeholder are sought and demonstrated as being considered and incorporated into the project design.</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>P.2.1.2</t>
+          <t>P.1.1.1</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>The project limits the participation of women or men based on pregnancy, maternity/paternity leave, or marital status.</t>
+          <t>The project developer, its representatives, and the project do not disrespect internationally proclaimed human rights.</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>P.2.1.2</t>
+          <t>P.1.1.1</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Information about project objectives is being communicated in a way that is inappropriate for the local context and not tailored to the methods of understanding of both women and men, which could hinder their participation.</t>
+          <t>The project is not involved or complicit in violence or human rights abuses of any kind as defined in the Universal Declaration of Human Rights.</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>P.2.1.3</t>
+          <t>P.1.1.2</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>The project has assessed gender risks without referencing the country's gender strategy or equivalent national commitment.</t>
+          <t>Local communities or individuals have not raised human rights concerns regarding the project.</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>P.2.1.4</t>
+          <t>P.1.1.3</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Expert stakeholder(s) have been involved, and their input has been requested for the project design on gender equality and women's empowerment.</t>
+          <t>There is no risk that rights-holders do not have the capacity to claim their rights.</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>P.2.1.1</t>
+          <t>P.1.1.3</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to adverse impacts on gender equality and/or the situation of women and girls.</t>
+          <t>This project does not undermine national or regional measures for the realization of the right to development.</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>P.2.1.1</t>
+          <t>P.1.1.1</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to exacerbation of risks of gender-based violence.</t>
+          <t>The project does not potentially involve or lead to adverse impacts on enjoyment of the human rights of the affected population, particularly of marginalized groups.</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>P.2.1.2</t>
+          <t>P.1.1.2</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to reproducing discriminations against women based on gender, especially regarding participation in design and implementation or access to opportunities and benefits.</t>
+          <t>The project does not potentially have inequitable or discriminatory impacts on affected populations, particularly people living in poverty or marginalized or excluded individuals or groups, including persons with disabilities.</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>P.2.1.2</t>
+          <t>P.1.1.3</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to limitations on women’s ability to use, develop and protect natural resources, taking into account different roles and positions of women and men in accessing environmental goods and services.</t>
+          <t>The project does not potentially lead to restrictions in availability, quality of and/or access to resources or basic services, in particular to marginalized groups.</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>P.3.1.1</t>
+          <t>P.1.1.3</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>The project involves potential risks to the health and safety of affected communities during its life cycle.</t>
+          <t>The project has restrictions in availability, quality of and/or access to resources or basic services, in particular to marginalised individuals or groups, including persons with disabilities.</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>P.3.1.2</t>
+          <t>P.1.1.3</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>The project involves any potential risks to the workers' safety and health.</t>
+          <t>The project exacerbates conflicts among and/or the risk of violence to project-affected communities and individuals.</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>P.3.1.1</t>
+          <t>P.2.1.1</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to construction and/or infrastructure development (e.g., roads, buildings, dams).</t>
+          <t>Women’s groups/leaders have raised gender equality concerns regarding the project during the stakeholder engagement process, grievance processes, or public statements.</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>P.3.1.2</t>
+          <t>P.2.1.2</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to air pollution, noise, vibration, traffic, injuries, physical hazards, poor surface water quality due to runoff, erosion, sanitation.</t>
+          <t>The project does not undermine the principles of non-discrimination, equal treatment, and equal pay for equal work.</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>P.3.1.2</t>
+          <t>P.2.1.2</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to harm or losses due to failure of structural elements of the project (e.g., collapse of buildings or infrastructure).</t>
+          <t>The project does not prevent men and women from having equal opportunities to participate in identified tasks and activities, whether through paid work, volunteer work, or community contributions, as appropriate.</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>P.3.1.2</t>
+          <t>P.2.1.2</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to risks of water-borne or other vector-borne diseases (e.g., temporary breeding habitats), communicable and noncommunicable diseases, nutritional disorders, mental health.</t>
+          <t>The project does not limit the participation of women or men based on pregnancy, maternity/paternity leave, or marital status.</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>P.3.1.2</t>
+          <t>P.2.1.2</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to transport, storage, and use and/or disposal of hazardous or dangerous materials (e.g., explosives, fuel and other chemicals during construction and operation).</t>
+          <t>Information about project objectives is communicated in a way that is appropriate for the local context and tailored to the methods of understanding of both women and men, which facilitates their participation.</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>P.3.1.2</t>
+          <t>P.2.1.3</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>There are adverse impacts on ecosystems and ecosystem services relevant to communities’ health.</t>
+          <t>The project has assessed gender risks referencing the country's gender strategy or equivalent national commitment.</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>P.4.1.1</t>
+          <t>P.2.1.4</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>The project involves altering, damaging, or removing sites, objects, or structures of significant cultural heritage.</t>
+          <t>Expert stakeholder(s) have been involved, and their input has been requested for the project design on gender equality and women's empowerment.</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>P.4.1.1</t>
+          <t>P.2.1.1</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>The project involves activities adjacent to or within a cultural heritage site.</t>
+          <t>The project potentially involves or leads to adverse impacts on gender equality and/or the situation of women and girls.</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>P.4.1.1</t>
+          <t>P.2.1.1</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>The project involves significant excavations, demolitions, movement of earth, flooding or other environmental changes.</t>
+          <t>The project potentially involves or leads to exacerbation of risks of gender-based violence.</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>P.4.1.1</t>
+          <t>P.2.1.2</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>The project involves alterations to landscapes and natural features with cultural significance.</t>
+          <t>The project potentially involves or leads to reproducing discriminations against women based on gender, especially regarding participation in design and implementation or access to opportunities and benefits.</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>P.4.1.1</t>
+          <t>P.2.1.2</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>The project has adverse impacts to sites, structures, or objects with historical, cultural, artistic, traditional or religious values or intangible forms of culture.</t>
+          <t>The project potentially involves or leads to limitations on women’s ability to use, develop and protect natural resources, taking into account different roles and positions of women and men in accessing environmental goods and services.</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>P.4.1.2</t>
+          <t>P.3.1.1</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>The project involves utilisation of tangible and/or intangible forms of Cultural Heritage for commercial or other purposes.</t>
+          <t>The project involves potential risks to the health and safety of affected communities during its life cycle.</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>P.4.1.2</t>
+          <t>P.3.1.2</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>If the project involves utilisation of Cultural Heritage for commercial or other purposes, the communities are made aware of their rights under the law, scope and nature of proposed development and its potential consequences.</t>
+          <t>The project involves any potential risks to the workers' safety and health.</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>P.4.1.3</t>
+          <t>P.3.1.1</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>If the project involves utilisation of Cultural Heritage for commercial purposes, it provides equitable sharing of benefits from commercialisation of such knowledge, innovation, or practice, consistent with their customs and traditions.</t>
+          <t>The project potentially involves or leads to construction and/or infrastructure development (e.g., roads, buildings, dams).</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>P.4.1.4</t>
+          <t>P.3.1.2</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>If the project involves utilisation of Cultural Heritage for commercial purposes, opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
+          <t>The project potentially involves or leads to air pollution, noise, vibration, traffic, injuries, physical hazards, poor surface water quality due to runoff, erosion, sanitation.</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>P.4.1.4</t>
+          <t>P.3.1.2</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>If the project involves utilisation of Cultural Heritage for commercial purposes, the project design has been changed, modified, updated considering opinions and recommendations of an Expert Stakeholder.</t>
+          <t>The project potentially involves or leads to harm or losses due to failure of structural elements of the project (e.g., collapse of buildings or infrastructure).</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>P.4.2.1</t>
+          <t>P.3.1.2</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>The project involves risks related to involuntary relocation of people.</t>
+          <t>The project potentially involves or leads to risks of water-borne or other vector-borne diseases (e.g., temporary breeding habitats), communicable and noncommunicable diseases, nutritional disorders, mental health.</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>P.4.2.1</t>
+          <t>P.3.1.2</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to risk of forced evictions or involuntary relocation of people.</t>
+          <t>The project potentially involves or leads to transport, storage, and use and/or disposal of hazardous or dangerous materials (e.g., explosives, fuel and other chemicals during construction and operation).</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>P.4.2.2</t>
+          <t>P.3.1.2</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to temporary or permanent and full or partial physical displacement, including people without legally recognisable claims to land.</t>
+          <t>The project potentially involves or leads to adverse impacts on ecosystems and ecosystem services relevant to communities’ health (e.g., food, surface water purification, natural buffers from flooding).</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>P.4.2.2</t>
+          <t>P.3.1.2</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to economic displacement, such as loss of assets or access to resources due to land acquisition or access restrictions, even in the absence of physical relocation.</t>
+          <t>The project addresses any identified risk related to community health and safety.</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>P.4.2.2</t>
+          <t>P.4.1.1</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>If the project potentially involves or leads to economic displacement, has the project developed Resettlement Action Plan or Livelihood Action Plan in consultation and agreement with affected individual, group or community, and integrated it into the Project design?</t>
+          <t>The project involves altering, damaging, or removing sites, objects, or structures of significant cultural heritage.</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>P.4.2.3</t>
+          <t>P.4.1.1</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>If the project potentially involves or leads to economic displacement, are opinions and recommendations of an Expert Stakeholder(s) not sought and demonstrated as being included in the project design?</t>
+          <t>The project potentially involves or leads to activities adjacent to or within a cultural heritage site.</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>P.4.2.3</t>
+          <t>P.4.1.1</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>If the project potentially involves or leads to economic displacement, have project design been changed, modified, updated considering opinions and recommendations of an Expert Stakeholder?</t>
+          <t>The project potentially involves significant excavations, demolitions, movement of earth, flooding or other environmental changes.</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>P.4.3.1</t>
+          <t>P.4.1.1</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>The project involves risks related to identifying and managing legitimate tenure rights that may be affected by the project.</t>
+          <t>The project potentially involves alterations to landscapes and natural features with cultural significance.</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>P.4.3.1</t>
+          <t>P.4.1.1</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to impacts on or changes to land tenure arrangements and/or community-based property rights/customary rights to land, territories and/or resources.</t>
+          <t>The project potentially has adverse impacts to sites, structures, or objects with historical, cultural, artistic, traditional or religious values or intangible forms of culture.</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>P.4.3.1</t>
+          <t>P.4.1.2</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to uncertainties with regards to land tenure, access rights, usage rights or land ownership.</t>
+          <t>The project utilizes tangible and/or intangible forms of Cultural Heritage for commercial or other purposes.</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>P.4.3.1</t>
+          <t>P.4.1.2</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>There are uncertainties with regards to land tenure, access rights, usage rights or land ownership.</t>
+          <t>The communities are made aware of their right under the law, scope and nature of proposed development and its potential consequences.</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>P.4.3.2</t>
+          <t>P.4.1.3</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Changes in legal arrangements are done in line with relevant laws and regulations.</t>
+          <t>The project provides equitable sharing of benefits from commercialization of such knowledge, innovation, or practice, consistent with their customs and traditions.</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>P.4.3.2</t>
+          <t>P.4.1.4</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Changes in legal arrangements agree with free, prior and informed consent of the involved stakeholders.</t>
+          <t>The opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>P.4.3.3</t>
+          <t>P.4.1.4</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Some other entity (other than the project developer) holds uncontested land title for the entire Project Boundary.</t>
+          <t>The project design has been changed, modified, updated considering opinions and recommendations of an Expert Stakeholder.</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>P.4.3.4</t>
+          <t>P.4.2.1</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
+          <t>The project involves risks related to involuntary relocation of people.</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>P.4.3.4</t>
+          <t>P.4.2.1</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>If opinions and recommendations of an Expert Stakeholder(s) are not sought, the project design has been changed, modified, updated considering opinions and recommendations of an Expert Stakeholder.</t>
+          <t>The project potentially involves or leads to risks of forced evictions or involuntary relocation of people.</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>P.4.3.5</t>
+          <t>P.4.2.2</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Project developer in consultation with stakeholders has established a functioning mechanism to receive, process, resolve, communicate and record grievances.</t>
+          <t>The project potentially involves or leads to temporary or permanent and full or partial physical displacement (including people without legally recognisable claims to land).</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>P.4.4.1</t>
+          <t>P.4.2.2</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>The project involves Indigenous People within the Project area of influence who may be affected directly or indirectly by the Project.</t>
+          <t>The project potentially involves or leads to economic displacement (e.g., loss of assets or access to resources due to land acquisition or access restrictions – even in the absence of physical relocation).</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>P.4.4.1</t>
+          <t>P.4.2.2</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to affect areas where indigenous peoples are present (including project area of influence).</t>
+          <t>The project has developed a Resettlement Action Plan or Livelihood Action Plan in consultation and agreement with affected individuals, groups, or communities.</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>P.4.4.1</t>
+          <t>P.4.2.3</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to affect areas, land and territory claimed by indigenous peoples.</t>
+          <t>The opinions and recommendations of Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>P.4.4.1</t>
+          <t>P.4.2.3</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to impacts (positive or negative) to the human rights, lands, natural resources, territories, and traditional livelihoods of indigenous peoples.</t>
+          <t>The project design has been changed, modified, or updated considering the opinions and recommendations of an Expert Stakeholder.</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>P.4.4.7</t>
+          <t>P.4.3.1</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>If the proposed project may affect the rights, lands, resources, or territories of indigenous people, an 'Indigenous People Plan' (IPP) or 'Indigenous People Plan Framework' has been elaborated and included in the project documentation, and was developed in accordance with the effective and meaningful participation of indigenous peoples and in accordance with UNDP Guidelines.</t>
+          <t>The project involves risks related to identifying and managing legitimate tenure rights that may be affected by the project.</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>P.4.4.3</t>
+          <t>P.4.3.1</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>The project has a risk of forcibly removing indigenous people from their lands and territories.</t>
+          <t>The project potentially involves or leads to impacts on or changes to land tenure arrangements and/or community-based property rights/customary rights to land, territories, and/or resources.</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>P.4.4.4</t>
+          <t>P.4.3.1</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>The project involves utilisation and/or commercial development of natural resources on lands and territories claimed by indigenous peoples.</t>
+          <t>The project potentially involves uncertainties with regards to land tenure, access rights, usage rights, or land ownership.</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>P.4.4.5</t>
+          <t>P.4.3.1</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>The project obtained free, prior and informed consent from indigenous people before taking their cultural, intellectual, religious, and/or spiritual property.</t>
+          <t>There are uncertainties with regards to land tenure, access rights, usage rights, or land ownership.</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>P.4.4.6</t>
+          <t>P.4.3.2</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>The project ensures that the indigenous people receive an equitable sharing of benefits resulting from the use of their traditional knowledge and practices.</t>
+          <t>Changes in legal arrangements are done in line with relevant laws and regulations.</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>P.4.4.8</t>
+          <t>P.4.3.2</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>The project lacks appropriate feedback and grievance channels for Indigenous Peoples and their representatives.</t>
+          <t>Changes in legal arrangements agree with free, prior and informed consent of the involved stakeholders.</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>P.4.4.8</t>
+          <t>P.4.3.3</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>A grievance mechanism has not been established at the beginning of programme or project implementation with due consideration given to customary dispute settlement mechanisms among the Indigenous Peoples concerned and will it remain operational throughout the project cycle.</t>
+          <t>Some other entity (other than the project developer) holds uncontested land title for the entire Project Boundary.</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>P.4.4.9</t>
+          <t>P.4.3.4</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
+          <t>Opinions and recommendations of an Expert Stakeholder(s) are sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>P.4.4.9</t>
+          <t>P.4.3.4</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>If the answer to the question about seeking opinions and recommendations of an Expert Stakeholder is 'YES', the project design has been changed, modified, updated considering opinions and recommendations of an Expert Stakeholder.</t>
+          <t>Project design has been changed, modified, or updated considering opinions and recommendations of an Expert Stakeholder.</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>P.5.1.1</t>
+          <t>P.4.3.5</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>The project involves, or is complicit in, contributing to or reinforcing corruption or corrupt projects.</t>
+          <t>The project developer in consultation with stakeholders has established a functioning mechanism to receive, process, resolve, communicate, and record grievances.</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>P.5.1.1</t>
+          <t>P.4.4.1</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>The project has a risk of encouraging bribery, kickbacks, or other unethical behavior.</t>
+          <t>The project involves Indigenous People within the Project area of influence who may be affected directly or indirectly by the Project.</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>P.6.1.1</t>
+          <t>P.4.4.1</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>The project involves, facilitates, or condones forced labor, or poses a potential risk of forced labor.</t>
+          <t>The project potentially involves or leads to affecting areas where indigenous peoples are present (including project area of influence).</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>P.6.1.1</t>
+          <t>P.4.4.1</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>The project violates any labor or health and safety laws, international obligations, or ILO conventions.</t>
+          <t>The project potentially affects areas, land, and territory claimed by indigenous peoples.</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>P.6.1.2</t>
+          <t>P.4.4.1</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>The project violates the principles of equal opportunity and fair treatment in its employment decisions.</t>
+          <t>The project potentially impacts (positive or negative) the human rights, lands, natural resources, territories, and traditional livelihoods of indigenous peoples.</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>P.6.1.3</t>
+          <t>P.4.4.7</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>The project violates national laws regarding non-discrimination in employment.</t>
+          <t>It is determined that the proposed project may affect the rights, lands, resources, or territories of indigenous people.</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>P.6.1.5</t>
+          <t>P.4.4.7</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>The project allows child labor.</t>
+          <t>An 'Indigenous People Plan' (IPP) or 'Indigenous People Plan Framework' has been elaborated and included in the project documentation.</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>P.6.1.8</t>
+          <t>P.4.4.7</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>The project has insufficient processes and measures in place to ensure the safety and health of project workers.</t>
+          <t>The plan was developed in accordance with the effective and meaningful participation of indigenous peoples and in accordance with UNDP Guidelines.</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>P.6.1.9</t>
+          <t>P.4.4.3</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>The project has insufficient measures to safeguard and support vulnerable project workers, such as women, people with disabilities, migrant workers, and young workers, and to prevent any kind of harassment, abuse, bullying, or exploitation, including gender-based violence (GBV).</t>
+          <t>The plan was developed in accordance with the effective and meaningful participation of indigenous peoples and in accordance with UNDP Guidelines.</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>P.6.1.10</t>
+          <t>P.4.4.4</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>The project has no grievance mechanism available for workers to voice workplace concerns, or information about this mechanism is not provided to workers at the time of recruitment, or it is not easily accessible.</t>
+          <t>The project has a risk of forcibly removing indigenous people from their lands and territories.</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>P.6.1.1</t>
+          <t>P.4.4.5</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to the use of forced labour.</t>
+          <t>The project involves the utilisation and/or commercial development of natural resources on lands and territories claimed by indigenous peoples.</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>P.6.1.1</t>
+          <t>P.4.4.6</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to working conditions that do not meet national labour laws and international commitments.</t>
+          <t>The project obtained free, prior and informed consent from indigenous people before taking their cultural, intellectual, religious, and/or spiritual property.</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>P.6.1.1</t>
+          <t>P.4.4.7</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>The project potentially involves or leads to working conditions that may deny freedom of association and collective bargaining.</t>
+          <t>The project ensures that the indigenous people receive an equitable sharing of benefits resulting from the use of their traditional knowledge and practices.</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>P.6.1.1</t>
+          <t>P.4.4.8</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>The developer ensures that migrant workers are engaged on substantially equivalent terms and conditions to non-migrant workers carrying out similar work.</t>
+          <t>The project ensures that the sharing of benefits resulting from the use of indigenous peoples' traditional knowledge and practices is culturally appropriate and inclusive.</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>P.6.1.1</t>
+          <t>P.4.4.9</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>The project developer puts in place and implements policies on the quality and management of accommodation and provision of basic services in a manner consistent with the principles of non-discrimination and equal opportunity.</t>
+          <t>The project ensures that the provision of equitable sharing of benefits does not impede land rights or equal access to basic services including health services, clean water, energy, education, safe and decent working conditions, and housing.</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>P.6.1.2</t>
+          <t>P.4.4.10</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>There is no form of discrimination or harassment based on factors unrelated to job requirements, such as gender, race, nationality, ethnicity, social or indigenous origin, religion or belief, disability, age, or sexual orientation.</t>
+          <t>The project lacks appropriate feedback and grievance channels for Indigenous Peoples and their representatives.</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>P.6.1.2</t>
+          <t>P.4.4.11</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>There is no form of discrimination in any aspect of employment, such as recruitment, compensation, working conditions, training, job assignment, promotion, termination, or discipline.</t>
+          <t>A grievance mechanism has not been established at the beginning of programme or project implementation with due consideration given to customary dispute settlement mechanisms among the Indigenous Peoples concerned and will it remain operational throughout the project cycle.</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>P.6.1.2</t>
+          <t>P.4.4.12</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>There is no harassment, intimidation, and/or exploitation, especially in regard to women.</t>
+          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>P.6.1.3</t>
+          <t>P.4.4.13</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>There are no discriminatory working conditions and/or lack of equal opportunity where national law provides provision to address non-discrimination in employment.</t>
+          <t>If the answer to the previous question is 'YES', project design has not been changed, modified, or updated considering opinions and recommendations of an Expert Stakeholder.</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>P.6.1.4</t>
+          <t>P.5.1.1</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>There is no use of child labour, including third-party engaged workers.</t>
+          <t>The project involves, or is it complicit in, contributing to or reinforcing corruption or corrupt projects.</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>P.6.1.4</t>
+          <t>P.5.1.2</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>There are inadequate and verifiable mechanisms for age verification.</t>
+          <t>The project has a risk of encouraging bribery, kickbacks, or other unethical behavior.</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>P.6.1.7</t>
+          <t>P.6.1.1</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>There are no processes and measures in place for the safety and health of project workers.</t>
+          <t>The project involves, facilitates, or condones forced labor, or poses a potential risk of forced labor.</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>P.6.1.7</t>
+          <t>P.6.1.1</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>There is no provision of safety and health training provisions, including on the proper use and maintenance of personal protective equipment conducted by competent persons and the maintenance of training records.</t>
+          <t>The project violates any labor or health and safety laws, international obligations, or ILO conventions.</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>P.6.1.7</t>
+          <t>P.6.1.2</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>There is no provision to record and document accidents, diseases, incidents, and any resulting injuries, illnesses, or deaths.</t>
+          <t>The project violates the principles of equal opportunity and fair treatment in its employment decisions.</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>P.6.1.8</t>
+          <t>P.6.1.3</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>There are occupational health and safety risks due to physical, chemical, biological and psychosocial hazards (including violence and harassment) throughout the project life-cycle.</t>
+          <t>The project violates national laws, if available regarding non-discrimination in employment.</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>P.6.1.9</t>
+          <t>P.6.1.5</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>There are no measures to protect vulnerable project workers from harassment, exploitation, and gender-based violence (GBV), including women, people with disabilities, migrant workers, and young workers.</t>
+          <t>The project allows child labor.</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>P.6.1.10</t>
+          <t>P.6.1.8</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>No grievance mechanism is available for workers to voice workplace concerns.</t>
+          <t>The project has insufficient processes and measures in place to ensure the safety and health of project workers.</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>P.6.1.11</t>
+          <t>P.6.1.9</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>No measures for due diligence and the establishment of policies and procedures to manage and monitor the performance of third-party employees in the project.</t>
+          <t>The project has insufficient measures to safeguard and support vulnerable project workers, such as women, people with disabilities, migrant workers, and young workers, and to prevent any kind of harassment, abuse, bullying, or exploitation, including gender-based violence (GBV).</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>P.6.2.1</t>
+          <t>P.6.1.10</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>There is a risk of project failure during implementation or after project certification due to a lack of financial resources.</t>
+          <t>The project has no grievance mechanism available for workers to voice workplace concerns, and information about this mechanism is not provided to workers at the time of recruitment, or is not easily accessible.</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>P.6.2.2</t>
+          <t>P.6.1.1</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>The project has potential negative impacts or poses a risk to the local economy.</t>
+          <t>The project potentially involves or leads to the use of forced labour.</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>P.6.2.2</t>
+          <t>P.6.1.1</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>There are potential risks or negative impacts this project may have on vulnerable or marginalised social groups, despite the benefits it may bring.</t>
+          <t>The project potentially involves or leads to working conditions that do not meet national labour laws and international commitments.</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>P.6.2.2</t>
+          <t>P.6.1.1</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>The project would involve or lead to economic impacts (negative/detrimental) to the local economy.</t>
+          <t>The project potentially involves or leads to working conditions that may deny freedom of association and collective bargaining.</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>P.6.2.2</t>
+          <t>P.6.1.1</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>The project would involve or lead to negative economic consequences during and after project implementation, e.g., for vulnerable and marginalised social groups in targeted communities.</t>
+          <t>The project developer shall provide reasonable working conditions and terms of employment if documented working agreements with all individual workers do not exist or do not address working conditions and terms of employment.</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>P.7.1.1</t>
+          <t>P.6.1.1</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>The project has a risk of increasing greenhouse gas emissions over the Baseline Scenario.</t>
+          <t>The developer shall ensure that migrant workers are engaged on substantially equivalent terms and conditions to non-migrant workers carrying out similar work if engaged.</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>P.7.1.1</t>
+          <t>P.6.1.1</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>The project would involve or lead to an increase in greenhouse gas emissions over the Baseline Scenario.</t>
+          <t>The project developer shall put in place and implement policies on the quality and management of the accommodation and provision of basic services in a manner consistent with the principles of non-discrimination and equal opportunity if there are no arrangements for basic services for workers.</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>P.7.2.1</t>
+          <t>P.6.1.2</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>The project poses a risk to the availability and reliability of energy supply to other users.</t>
+          <t>There is no form of discrimination or harassment based on factors unrelated to job requirements, such as gender, race, nationality, ethnicity, social or indigenous origin, religion or belief, disability, age, or sexual orientation.</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>P.7.2.1</t>
+          <t>P.6.1.2</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>The project poses a risk to the availability and reliability of energy supply to other users.</t>
+          <t>There is no form of discrimination in any aspect of employment, such as recruitment, compensation, working conditions, training, job assignment, promotion, termination, or discipline.</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>P.7.2.1</t>
+          <t>P.6.1.2</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>The project involves or leads to a negative impact on the availability and reliability of energy supply to other users.</t>
+          <t>There is no harassment, intimidation, and/or exploitation, especially in regard to women.</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>P.8.1.1</t>
+          <t>P.6.1.3</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>The project increases water usage to a level that will not allow for the maintenance of environmental flows.</t>
+          <t>There are no discriminatory working conditions and/or lack of equal opportunity where national law provides provision to address non-discrimination in employment.</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>P.8.1.1</t>
+          <t>P.6.1.4</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>The project results in the discharge of wastewater that does not meet the required standard for beneficial reuse and could therefore negatively impact the environmental flow.</t>
+          <t>There is no use of child labour, including third-party engaged workers.</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>P.8.1.1</t>
+          <t>P.6.1.4</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>The project has the potential risk to exceed the rate of recharge for the groundwater source.</t>
+          <t>There are adequate and verifiable mechanisms for age verification.</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>P.8.1.1</t>
+          <t>P.6.1.7</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>The project involves any processes or activities that could contaminate the groundwater and render it unsuitable for use.</t>
+          <t>There are processes and measures in place for the safety and health of project workers.</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>P.8.1.1</t>
+          <t>P.6.1.7</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>The project affects the natural or pre-existing pattern of watercourses, groundwater and/or the watershed(s) such as high seasonal flow variability, flooding potential, lack of aquatic connectivity or water scarcity.</t>
+          <t>There are provisions for safety and health training, including on the proper use and maintenance of personal protective equipment conducted by competent persons and the maintenance of training records.</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>P.8.1.1</t>
+          <t>P.6.1.7</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>The project involves wastewater discharge of quality that does not meet the required standard for beneficial reuse.</t>
+          <t>There is a provision to record and document accidents, diseases, incidents, and any resulting injuries, illnesses, or deaths.</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>P.8.1.1</t>
+          <t>P.6.1.8</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>The project involves significant extraction, diversion of ground water, such as construction of dams, reservoirs, river basin developments, groundwater extraction.</t>
+          <t>There are no occupational health and safety risks due to physical, chemical, biological and psychosocial hazards (including violence and harassment) throughout the project life-cycle.</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>P.8.1.2</t>
+          <t>P.6.1.9</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
+          <t>There are measures to protect vulnerable project workers from harassment, exploitation, and gender-based violence (GBV), including women, people with disabilities, migrant workers, and young workers.</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>P.8.2.1</t>
+          <t>P.6.1.10</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>The project has a risk of negatively impacting the catchment and has it been assessed and addressed.</t>
+          <t>There is a grievance mechanism available for workers to voice concerns.</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>P.8.2.1</t>
+          <t>P.6.1.10</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>The project has a risk of negatively impacting the catchment and it has been assessed and addressed.</t>
+          <t>No grievance mechanism is available for workers to voice workplace concerns.</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>P.8.2.5</t>
+          <t>P.6.1.11</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>The project would negatively impact the catchment area.</t>
+          <t>No measures for due diligence and the establishment of policies and procedures to manage and monitor the performance of third-party employees in the project.</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>P.8.2.6</t>
+          <t>P.6.2.1</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
+          <t>There is a risk of project failure during implementation or after project certification due to a lack of financial resources.</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>P.9.1.3</t>
+          <t>P.6.2.2</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>There is a risk of soil resource degradation or loss of ecosystem services provided by soils in the project.</t>
+          <t>The project has potential negative impacts or poses a risk to the local economy.</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>P.9.1.4</t>
+          <t>P.6.2.2</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>The project involves or leads to production, harvesting, and/or management of living natural resources by small-scale landholders and/or local communities.</t>
+          <t>There are potential risks or negative impacts this project may have on vulnerable or marginalised social groups, despite the benefits it may bring.</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>P.9.1.4</t>
+          <t>P.6.2.2</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>If the project involves or leads to production, harvesting, and/or management of living natural resources by small-scale landholders and/or local communities, the project adopts appropriate and culturally sensitive sustainable resource management practices.</t>
+          <t>The project would involve or lead to economic impacts (negative/detrimental) to the local economy.</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>P.9.2.1</t>
+          <t>P.6.2.2</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>The project has risks associated with natural or man-made hazards that could result from land use changes due to the project.</t>
+          <t>The project would lead to negative economic consequences during and after project implementation, e.g., for vulnerable and marginalised social groups in targeted communities.</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>P.9.2.1</t>
+          <t>P.7.1.1</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>The project has risks associated with natural or man-made hazards that could result from land use changes due to the project.</t>
+          <t>The project has a risk of increasing greenhouse gas emissions over the Baseline Scenario.</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>P.9.2.2</t>
+          <t>P.7.1.1</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>The project involves or leads to any potential risks that require emergency preparedness and response planning.</t>
+          <t>The project would involve or lead to an increase in greenhouse gas emissions over the Baseline Scenario.</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>P.9.2.2</t>
+          <t>P.7.2.1</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>If the project involves or leads to potential risks that require emergency preparedness and response planning, the project developer disclosed appropriate information about emergency preparedness and response to affected communities.</t>
+          <t>The project poses a risk to the availability and reliability of energy supply to other users.</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>P.9.3.1</t>
+          <t>P.7.2.1</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>The project involves the transfer, handling, and use of genetically modified organisms/living modified organisms that may result in adverse effects on biological diversity.</t>
+          <t>The project poses a risk to the availability and reliability of energy supply to other users.</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>P.9.3.1</t>
+          <t>P.7.2.1</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>The project involves or leads to the transfer, handling, and use of genetically modified organisms/living modified organisms (GMOs/LMOs) that result from modern biotechnology.</t>
+          <t>The project would involve or lead to a negative impact on the availability and reliability of energy supply to other users.</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>P.9.3.1</t>
+          <t>P.8.1.1</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>If the project involves or leads to the transfer, handling, and use of GMOs/LMOs, a risk assessment by a competent expert stakeholder has been carried out in accordance with Annex III of the Cartagena Protocol on Biosafety to the Convention on Biological Diversity.</t>
+          <t>The project increases water usage to a level that will not allow for the maintenance of environmental flows.</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>P.9.3.2</t>
+          <t>P.8.1.1</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>If a risk assessment has been carried out, any risks identified in the risk assessment.</t>
+          <t>The project results in the discharge of wastewater that does not meet the required standard for beneficial reuse and could therefore negatively impact the environmental flow.</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>P.9.3.3</t>
+          <t>P.8.1.1</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Forestry projects (for example Afforestation/Reforestation) involving GMO planting.</t>
+          <t>The project has the potential risk to exceed the rate of recharge for the groundwater source.</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>P.9.4.1</t>
+          <t>P.8.1.1</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>The project has a risk of releasing pollutants to air, water, and land in routine, non-routine, or accidental circumstances.</t>
+          <t>The project involves any processes or activities that could contaminate the groundwater and render it unsuitable for use.</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>P.9.4.1</t>
+          <t>P.8.1.1</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>The project involves or leads to any potential risk of pollutant release that cannot be avoided.</t>
+          <t>The project would involve or lead to affecting the natural or pre-existing pattern of watercourses, groundwater and/or the watershed(s) such as high seasonal flow variability, flooding potential, lack of aquatic connectivity or water scarcity.</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>P.9.4.3</t>
+          <t>P.8.1.1</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>The project has identified all potential pollution sources that may degrade the quality of soil, air, surface, and groundwater in the project area.</t>
+          <t>The project would involve or lead to wastewater discharge of quality that does not meet the required standard for beneficial reuse.</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>P.9.4.2</t>
+          <t>P.8.1.1</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>The pollution prevention and control technologies and practices applied during the project life cycle align with national regulations or international best practices.</t>
+          <t>The project would involve or lead to significant extraction, diversion of groundwater.</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>P.9.4.3</t>
+          <t>P.8.1.2</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>There is a monitoring plan to ensure that mitigation measures are implemented, and resources are protected.</t>
+          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>P.9.5.1</t>
+          <t>P.8.2.1</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>The project involves the generation of waste materials (both hazardous and non-hazardous).</t>
+          <t>The project has a risk of negatively impacting the catchment and has it been assessed and addressed.</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>P.9.5.3</t>
+          <t>P.8.2.1</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>The project involves risk of release of hazardous materials resulting from their production, transportation, handling, storage, or use.</t>
+          <t>The project has a risk of negatively impacting the catchment and has been assessed and addressed.</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>P.9.5.5</t>
+          <t>P.8.2.5</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>The project involves the use of any chemicals or materials subject to international bans or phase-outs.</t>
+          <t>The project negatively impacts on the catchment area.</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>P.9.5.1</t>
+          <t>P.8.2.6</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>The project involves the generation and management of waste materials.</t>
+          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>P.9.5.1</t>
+          <t>P.9.1.3</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>The project involves treatment, destruction, or disposal of waste material.</t>
+          <t>There is a risk of soil resource degradation or loss of ecosystem services provided by soils in the project.</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>P.9.5.1</t>
+          <t>P.9.1.4</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>The project involves an environmentally friendly method that includes appropriate control of emissions and residues resulting from the handling and processing of waste material.</t>
+          <t>The project involves or leads to production, harvesting, and/or management of living natural resources by small-scale landholders and/or local communities.</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>P.9.5.3</t>
+          <t>P.9.1.4</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>The project involves risk of release of hazardous materials resulting from their production, transportation, handling, storage, or use.</t>
+          <t>If the answer to the above question is 'yes' or 'potentially', the project adopts appropriate and culturally sensitive sustainable resource management practices.</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>P.9.5.3</t>
+          <t>P.9.2.1</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>The project has measures in place to address health risks.</t>
+          <t>The project has risks associated with natural or man-made hazards that could result from land use changes due to the project.</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>P.9.5.4</t>
+          <t>P.9.2.1</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>The project involves manufacture, trade, and use of chemicals and hazardous materials subject to international bans or phase-outs due to their high toxicity to living organisms, environmental persistence, potential for bioaccumulation, or potential for depletion of the ozone layer.</t>
+          <t>The project has risks associated with natural or man-made hazards that could result from land use changes due to the project.</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>P.9.6.1</t>
+          <t>P.9.2.2</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>The project involves the use of chemical pesticides.</t>
+          <t>The project involves or leads to potential risks that require emergency preparedness and response planning.</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>P.9.6.5</t>
+          <t>P.9.2.2</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>The project involves purchase, store, manufacture, trade or use products that fall in Classes IA (extremely hazardous) and IB (highly hazardous).</t>
+          <t>If the answer to the above question is 'yes' or 'potentially', the project developer disclosed appropriate information about emergency preparedness and response to affected communities.</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>P.9.6.6</t>
+          <t>P.9.3.1</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>The project uses fertilisers, and measures are being taken to minimise their use and nutrient losses to the environment.</t>
+          <t>The project involves the transfer, handling, and use of genetically modified organisms/living modified organisms that may result in adverse effects on biological diversity.</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>P.9.6.1</t>
+          <t>P.9.3.1</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>The project involves chemical pesticides use for pest management.</t>
+          <t>The project involves the transfer, handling and use of genetically modified organisms/living modified organisms (GMOs/LMOs) that result from modern biotechnology.</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>P.9.6.4</t>
+          <t>P.9.3.1</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>If the answer to the question above is 'yes' or 'potentially', the project has a documented Chemical Pesticides Policy in place.</t>
+          <t>If the answer to the above question is 'yes', a risk assessment by a competent Expert stakeholder has been carried out in accordance with Annex iii of the Cartagena protocol on biosafety to the convention on biological diversity.</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>P.9.6.5</t>
+          <t>P.9.3.2</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>The project involves purchase, store, use, manufacture, or trade in Class II (moderately hazardous) pesticides.</t>
+          <t>If the answer to the above question is 'yes', any risks identified in the risk assessment.</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>P.9.6.5</t>
+          <t>P.9.3.3</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>If the answer to the question above is 'yes' or 'potentially', the project has appropriate controls on manufacture, procurement, or distribution and/or use of these chemicals.</t>
+          <t>The project involves Forestry (for example Afforestation/Reforestation) involving GMO planting.</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>P.9.7.1</t>
+          <t>P.9.4.1</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>The project has a risk of unsustainable forest management, including timber harvesting.</t>
+          <t>The project has a risk of releasing pollutants to air, water, and land in routine, non-routine, or accidental circumstances.</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>P.9.7.1</t>
+          <t>P.9.4.1</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>The project poses a risk of depleting biodiversity and ecosystem functionality in areas where improved forest management is undertaken.</t>
+          <t>The project involves or leads to any potential risk of pollutant release that cannot be avoided.</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>P.9.7.1</t>
+          <t>P.9.4.3</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>The project risks not meeting requirements for environment-friendly, socially beneficial, and economically viable plantations using native species whenever possible.</t>
+          <t>If the answer to the above question is 'Yes' or 'potentially', the project has identified all potential pollution sources that may degrade the quality of soil, air, surface, and groundwater in the project area.</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>P.9.8.1</t>
+          <t>P.9.4.2</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>The project involves the risk of negatively influencing access to and availability of food for people affected.</t>
+          <t>If the answer to the above question is 'Yes' or 'potentially', the pollution prevention and control technologies and practices applied during the project life cycle align with national regulations or international best practices.</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>P.9.8.1</t>
+          <t>P.9.4.3</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>The project involves or leads to modification of the quantity or nutritional quality of food available such as through crop regime alteration or export or economic incentives.</t>
+          <t>If the answer to the above question is 'Yes', there is a monitoring plan to ensure that mitigation measures are implemented, and resources are protected.</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>P.9.9.1</t>
+          <t>P.9.5.1</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>The project involves any risks to animal welfare.</t>
+          <t>The project involves the generation of waste materials (both hazardous and non-hazardous).</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>P.9.9.2</t>
+          <t>P.9.5.3</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>The project involves any potential risk of excessive or inadequate use of veterinary medicines.</t>
+          <t>The project involves risk of release of hazardous materials resulting from their production, transportation, handling, storage, or use.</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>P.9.9.4</t>
+          <t>P.9.5.5</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>The project involves the risk of administering synthetic growth promoters, including hormones.</t>
+          <t>The project involves the use of any chemicals or materials subject to international bans or phase-outs.</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>P.9.9.1</t>
+          <t>P.9.5.1</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>The project involves or leads to animal husbandry or harvesting of fish populations or other aquatic species.</t>
+          <t>The project involves the generation and management of waste materials.</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>P.9.9.1</t>
+          <t>P.9.5.1</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>The project involves or leads to limiting access for animals to basic needs like drinking water, adequate food, daylight, appropriate shelter etc.</t>
+          <t>The project involves treatment, destruction, or disposal of waste material.</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>P.9.9.3</t>
+          <t>P.9.5.1</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>The project involves inadequate measures to isolate sick animals and control the spread of disease, especially zoonotic diseases.</t>
+          <t>If the answer to the above question is 'Yes', the project involves an environmentally friendly method that includes appropriate control of emissions and residues resulting from the handling and processing of waste material.</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>P.9.9.5</t>
+          <t>P.9.5.3</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>The project involves inadequate low-stress methods, equipment, and facilities that facilitate calm animal movement.</t>
+          <t>The project involves risk of release of hazardous materials resulting from their production, transportation, handling, storage, or use.</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>P.9.9.6</t>
+          <t>P.9.5.3</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>The project involves inadequate measures to ensure that animals are exposed to the least stress possible during transportation and slaughtering.</t>
+          <t>If the answer to the above question is 'yes', the project has measures in place to address health risks.</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>P.9.9.7</t>
+          <t>P.9.5.4</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>The project involves inappropriate spacing per animal and stocking rates per land unit.</t>
+          <t>The project involves manufacture, trade, and use of chemicals and hazardous materials subject to international bans or phase-outs due to their high toxicity to living organisms.</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>P.9.9.8</t>
+          <t>P.9.6.1</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>The project involves inadequate measures to address the specific needs of aquatic animals.</t>
+          <t>The project involves the use of chemical pesticides.</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>P.9.9.8</t>
+          <t>P.9.6.5</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>There are inadequate measures to address the specific needs of aquatic animals.</t>
+          <t>The project involves purchase, store, manufacture, trade or use products that fall in Classes IA (extremely hazardous) and IB (highly hazardous).</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>P.9.9.10</t>
+          <t>P.9.6.6</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>The primary production of living natural resources such as animal husbandry, aquaculture, and fisheries is involved.</t>
+          <t>The project uses fertilisers, and measures are being taken to minimise their use and nutrient losses to the environment.</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>P.9.10.1</t>
+          <t>P.9.6.1</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>The project has the risk of negatively impacting HCV areas and/or critical habitats.</t>
+          <t>The project involves chemical pesticides use for pest management.</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>P.9.10.2</t>
+          <t>P.9.6.4</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>The project in the project area or area of downstream impacts has risks to native tree patches, individual native trees, freshwater resources, habitats of rare, threatened, and endangered species, and biodiversity-enhancing areas.</t>
+          <t>The project has a documented Chemical Pesticides Policy in place.</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>P.9.10.1</t>
+          <t>P.9.6.5</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>The project involves or leads to identified habitats as HCV areas and or Critical habitats.</t>
+          <t>The project involves purchase, store, use, manufacture, or trade in Class II (moderately hazardous) pesticides.</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>P.9.10.1</t>
+          <t>P.9.6.5</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>If the project involves identified habitats as HCV areas and or Critical habitats, the project has risks that could negatively impact the catchment, project success, and surrounding HCV and ecological assets, as well as any measurable adverse impacts on the criteria or biodiversity values for which the critical habitat was designated, and on the ecological processes supporting that biodiversity.</t>
+          <t>The project has appropriate controls on manufacture, procurement, or distribution and/or use of these chemicals.</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>P.9.10.1</t>
+          <t>P.9.7.1</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>If the project involves identified habitats as HCV areas and or Critical habitats, a robust, appropriately designed, and long-term Habitats and Biodiversity Action Plan is absent which will make the project unable to achieve net gains of those biodiversity values for which the critical habitat was designated.</t>
+          <t>The project has a risk of unsustainable forest management, including timber harvesting.</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>P.9.10.2</t>
+          <t>P.9.7.1</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>The project area or area of downstream impacts has native tree patches, individual native trees, freshwater resources, habitats of rare, threatened, and endangered species, and biodiversity-enhancing areas.</t>
+          <t>The project poses a risk of depleting biodiversity and ecosystem functionality in areas where improved forest management is undertaken.</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>P.9.10.2</t>
+          <t>P.9.7.1</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>If the project area or area of downstream impacts has native tree patches, individual native trees, freshwater resources, habitats of rare, threatened, and endangered species, and biodiversity-enhancing areas, the project will have any adverse effects on these areas.</t>
+          <t>The project risks not meeting requirements for environment-friendly, socially beneficial, and economically viable plantations using native species whenever possible.</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>P.9.10.3</t>
+          <t>P.9.8.1</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>The project has opportunities to minimise unwarranted conversion or degradation of the habitat and to enhance the habitat as part of its development.</t>
+          <t>The project involves the risk of negatively influencing access to and availability of food for people affected.</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>P.9.10.4</t>
+          <t>P.9.8.1</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>The project is applying Land Use &amp; Forest Activity Requirements and managing a minimum 10% of the project area to protect or enhance the biological diversity of native ecosystems following HCV approach as per the given requirements.</t>
+          <t>The project involves or leads to modification of the quantity or nutritional quality of food available such as through crop regime alteration or export or economic incentives.</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>P.9.10.5</t>
+          <t>P.9.9.1</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
+          <t>The project involves any risks to animal welfare.</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>P.9.11.1</t>
+          <t>P.9.9.2</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>The project leads to the reduction or negative impact on any recognised Endangered, Vulnerable or Critically Endangered species.</t>
+          <t>The project involves any potential risk of excessive or inadequate use of veterinary medicines.</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>P.9.11.2</t>
+          <t>P.9.9.4</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>The project involves or leads to distortion of habitats of endangered species.</t>
+          <t>The project involves the risk of administering synthetic growth promoters, including hormones.</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>P.9.11.2</t>
+          <t>P.9.9.1</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>The project plans to protect and enhance habitats of endangered species if distortion occurs.</t>
+          <t>The project involves animal husbandry or harvesting of fish populations or other aquatic species.</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>P.9.11.2</t>
+          <t>P.9.9.1</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
+          <t>The project involves limiting access for animals to basic needs like drinking water, adequate food, daylight, appropriate shelter etc.</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>P.9.12.1</t>
+          <t>P.9.9.3</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>The project introduces any alien species (not currently established in the country or region of the project) into new environments.</t>
+          <t>The project involves inadequate measures to isolate sick animals and control the spread of disease, especially zoonotic diseases.</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>P.9.12.1</t>
+          <t>P.9.9.5</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>The project involves or leads to the risk of introducing any alien species with a high risk of invasive behaviour regardless of whether such introductions are permitted under the existing regulatory framework.</t>
+          <t>The project involves inadequate low-stress methods, equipment, and facilities that facilitate calm animal movement.</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>P.9.12.1</t>
+          <t>P.9.9.6</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>There is a risk of potential accidental or unintended introductions including the transportation of substrates and vectors that may harbour alien species.</t>
+          <t>The project involves inadequate measures to ensure that animals are exposed to the least stress possible during transportation and slaughtering.</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
+          <t>P.9.9.7</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>The project involves inappropriate spacing per animal and stocking rates per land unit.</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>P.9.9.8</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>The project involves inadequate measures to address the specific needs of aquatic animals.</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>P.9.10.1</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>The project has the risk of negatively impacting HCV areas and/or critical habitats.</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>P.9.10.2</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>The project in the project area or area of downstream impacts has risks to native tree patches, individual native trees, freshwater resources, habitats of rare, threatened, and endangered species, and biodiversity-enhancing areas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>P.9.10.1</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>The project involves or leads to identified habitats as HCV areas and/or Critical habitats.</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>P.9.10.1</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>If the answer to the above question is 'yes', the project has any risks that could negatively impact the catchment, project success, and surrounding HCV and ecological assets.</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>P.9.10.1</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>If the answer to the above question is 'yes', a robust, appropriately designed, and long-term Habitats and Biodiversity Action Plan is absent which will make the project unable to achieve net gains of those biodiversity values for which the critical habitat was designated.</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>P.9.10.2</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>The project area or area of downstream impacts has native tree patches, individual native trees, freshwater resources, habitats of rare, threatened, and endangered species, and biodiversity-enhancing areas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>P.9.10.2</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>If the answer to the above question is 'yes', the project will have any adverse effects on these areas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>P.9.10.3</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>If the answer to the above question is 'yes', the project has opportunities to minimize unwarranted conversion.</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>P.9.10.3</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>The project has opportunities to minimize unwarranted conversion or degradation of the habitat and to enhance the habitat as part of its development.</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>P.9.10.4</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>The project is applying Land Use &amp; Forest Activity Requirements and managing a minimum 10% of the project area to protect or enhance the biological diversity of native ecosystems following HCV approach as per the given requirements.</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>P.9.10.5</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Opinions and recommendations of an Expert Stakeholder(s) are not sought and demonstrated as being included in the project design.</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>P.9.11.1</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>The project leads to the reduction or negative impact on any recognised Endangered, Vulnerable or Critically Endangered species.</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>P.9.11.2</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>The project would involve or lead to distortion of habitats of endangered species.</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>P.9.11.2</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>If the answer to the above question is 'yes', the project plans to protect and enhance them.</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>P.9.12.1</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>The project introduces any alien species (not currently established in the country or region of the project) into new environments.</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>P.9.12.1</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>The project would involve or lead to risk of introducing any alien species with a high risk of invasive behaviour regardless of whether such introductions are permitted under the existing regulatory framework.</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>P.9.12.1</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>The project assesses the risk of potential accidental or unintended introductions including the transportation of substrates and vectors that may harbour alien species.</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
           <t>P.9.12.2</t>
         </is>
       </c>
-      <c r="B312" t="inlineStr">
-        <is>
-          <t>There is a risk of spreading alien species into areas in which they have not already been established.</t>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>The project assesses the risk of spreading alien species into areas in which they have not already been established.</t>
         </is>
       </c>
     </row>

</xml_diff>